<commit_message>
reiterated the scanning and processing of the scanning
now the scanning functions on individual scans rather than creating a transaction with the scans. Which allows the application to interact with each scan rather than being put into sleep mode until the keylogger-scanner session ends.
</commit_message>
<xml_diff>
--- a/SKU-Source-File.xlsx
+++ b/SKU-Source-File.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{796B0679-291D-416B-B79F-161D3A0A1211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB041D43-62E0-4691-925D-52F486547973}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28620" yWindow="0" windowWidth="28440" windowHeight="15195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="9810" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -1528,14 +1528,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40F0000C-532D-471E-BBDD-63A924EC574C}">
   <dimension ref="A1:D93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="A95" sqref="A95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="164" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.5703125" customWidth="1"/>
     <col min="3" max="3" width="39.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>